<commit_message>
Removed line breaks in header cells.
</commit_message>
<xml_diff>
--- a/samples/assets/pfw/CKEditor4.PFW.Balance.Sheet.xlsx
+++ b/samples/assets/pfw/CKEditor4.PFW.Balance.Sheet.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annatomanek/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.20.89\share\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="260" yWindow="800" windowWidth="28800" windowHeight="15960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7590" windowHeight="5130" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -29,14 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
-    <t>Full Year
-(unadited)</t>
-  </si>
-  <si>
-    <t>2013
-(unadited)</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -182,6 +171,12 @@
   </si>
   <si>
     <t>$2,255</t>
+  </si>
+  <si>
+    <t>Full Year (unadited)</t>
+  </si>
+  <si>
+    <t>2013 (unadited)</t>
   </si>
 </sst>
 </file>
@@ -285,15 +280,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -306,19 +298,25 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hiperłącze" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperłącze" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperłącze" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperłącze" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperłącze" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Odwiedzone hiperłącze" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Odwiedzone hiperłącze" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Odwiedzone hiperłącze" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Odwiedzone hiperłącze" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Odwiedzone hiperłącze" xfId="10" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -332,6 +330,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -603,233 +604,233 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="55.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="19.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3">
+        <v>2011</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2012</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2013</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="4">
-        <v>2011</v>
-      </c>
-      <c r="C2" s="4">
-        <v>2012</v>
-      </c>
-      <c r="D2" s="4">
-        <v>2013</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="4" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="6" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>9</v>
+      <c r="C4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="6" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="B5" s="5">
+        <v>52</v>
+      </c>
+      <c r="C5" s="5">
+        <v>54</v>
+      </c>
+      <c r="D5" s="5">
+        <v>53</v>
+      </c>
+      <c r="E5" s="5">
+        <v>45</v>
+      </c>
+      <c r="F5" s="5">
+        <v>47</v>
+      </c>
+      <c r="G5" s="5">
+        <v>47</v>
+      </c>
+      <c r="H5" s="5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>16</v>
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="6">
-        <v>52</v>
-      </c>
-      <c r="C5" s="6">
-        <v>54</v>
-      </c>
-      <c r="D5" s="6">
-        <v>53</v>
-      </c>
-      <c r="E5" s="6">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="6">
-        <v>47</v>
-      </c>
-      <c r="H5" s="6">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -838,6 +839,6 @@
     <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed a typo in Excel file.
</commit_message>
<xml_diff>
--- a/samples/assets/pfw/CKEditor4.PFW.Balance.Sheet.xlsx
+++ b/samples/assets/pfw/CKEditor4.PFW.Balance.Sheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7590" windowHeight="5130" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9255" windowHeight="2595" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -173,16 +173,16 @@
     <t>$2,255</t>
   </si>
   <si>
-    <t>Full Year (unadited)</t>
-  </si>
-  <si>
-    <t>2013 (unadited)</t>
+    <t>Full Year (unaudited)</t>
+  </si>
+  <si>
+    <t>2013 (unaudited)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -306,17 +306,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="11">
-    <cellStyle name="Hiperłącze" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperłącze" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperłącze" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperłącze" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperłącze" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Paste from Excel sample updated.
</commit_message>
<xml_diff>
--- a/samples/assets/pfw/CKEditor4.PFW.Balance.Sheet.xlsx
+++ b/samples/assets/pfw/CKEditor4.PFW.Balance.Sheet.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.20.89\share\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annatomanek/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9255" windowHeight="2595" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="24440" windowHeight="13700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -182,7 +185,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -267,8 +270,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -305,17 +318,27 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -603,17 +626,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="55.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.125" customWidth="1"/>
+    <col min="1" max="1" width="51.6640625" style="1" customWidth="1"/>
+    <col min="2" max="8" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="8" t="s">
         <v>49</v>
@@ -651,7 +674,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -677,7 +700,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -703,7 +726,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
@@ -729,7 +752,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
@@ -755,7 +778,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>26</v>
       </c>
@@ -781,7 +804,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
@@ -807,7 +830,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>

</xml_diff>